<commit_message>
Correct cargo dist conversion factor
</commit_message>
<xml_diff>
--- a/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
+++ b/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\web-app\CDCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\web-app\CDCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA71D1-6D81-4008-A213-EFDB3EA69279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47D5282-DBE5-42DA-9427-489704DC73EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9320" yWindow="40" windowWidth="15660" windowHeight="13700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="CDCF-PMpPDOU" sheetId="2" r:id="rId2"/>
     <sheet name="CDCF-FTMpFDOU" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -56,12 +56,6 @@
     <t>For the U.S. model, the desired output units are:</t>
   </si>
   <si>
-    <t>trillion passenger-miles</t>
-  </si>
-  <si>
-    <t>trillion freight ton-miles</t>
-  </si>
-  <si>
     <t>CDCF Passenger Miles per Passenger Distance Output Unit</t>
   </si>
   <si>
@@ -80,7 +74,13 @@
     <t>CDCF Freight Ton Miles per Freight Distance Output Unit</t>
   </si>
   <si>
-    <t>miles to kilometers</t>
+    <t>milliom passenger-miles</t>
+  </si>
+  <si>
+    <t>million freight ton-miles</t>
+  </si>
+  <si>
+    <t>km to miles</t>
   </si>
 </sst>
 </file>
@@ -471,23 +471,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,47 +495,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>1.60934</v>
+        <f>1/1.60934</f>
+        <v>0.62137273664980675</v>
       </c>
     </row>
   </sheetData>
@@ -552,27 +553,27 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <f>10^12*About!$B$15</f>
-        <v>1609340000000</v>
+        <f>10^6*About!$B$15</f>
+        <v>621372.73664980673</v>
       </c>
     </row>
   </sheetData>
@@ -587,28 +588,28 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <f>10^12*About!$B$15</f>
-        <v>1609340000000</v>
+        <f>10^6*About!$B$15</f>
+        <v>621372.73664980673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>